<commit_message>
Status Report 3 + EVM Update
Co-Authored-By: angeloafeltra <73121300+angeloafeltra@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Documenti/EVM/GreenLeaf_EVM.xlsx
+++ b/Documenti/EVM/GreenLeaf_EVM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11211"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\Documents\Green-Leaf\Documenti\EVM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antoniogiametta/Documents/GitHub/Green-Leaf/Documenti/EVM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855D4CE1-B021-4418-A834-8800F86B95FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3269627-72E9-904B-8279-4D997FE25A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" tabRatio="261" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="27860" windowHeight="17500" tabRatio="261" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="definizioni" sheetId="1" r:id="rId1"/>
@@ -304,16 +304,16 @@
     <t>09/12/2022</t>
   </si>
   <si>
-    <t>23/12/2022</t>
-  </si>
-  <si>
-    <t>23/01/20232</t>
-  </si>
-  <si>
-    <t>24/01/2023</t>
-  </si>
-  <si>
-    <t>26/01/2023</t>
+    <t>30/12/22</t>
+  </si>
+  <si>
+    <t>23/01/23</t>
+  </si>
+  <si>
+    <t>25/01/23</t>
+  </si>
+  <si>
+    <t>26/01/23</t>
   </si>
 </sst>
 </file>
@@ -1531,16 +1531,16 @@
                   <c:v>09/12/2022</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23/12/2022</c:v>
+                  <c:v>30/12/22</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23/01/20232</c:v>
+                  <c:v>23/01/23</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24/01/2023</c:v>
+                  <c:v>25/01/23</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>26/01/2023</c:v>
+                  <c:v>26/01/23</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1561,7 +1561,7 @@
                   <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>10.285714285714286</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1634,16 +1634,16 @@
                   <c:v>09/12/2022</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23/12/2022</c:v>
+                  <c:v>30/12/22</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23/01/20232</c:v>
+                  <c:v>23/01/23</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24/01/2023</c:v>
+                  <c:v>25/01/23</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>26/01/2023</c:v>
+                  <c:v>26/01/23</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1978,16 +1978,16 @@
                   <c:v>09/12/2022</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23/12/2022</c:v>
+                  <c:v>30/12/22</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23/01/20232</c:v>
+                  <c:v>23/01/23</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24/01/2023</c:v>
+                  <c:v>25/01/23</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>26/01/2023</c:v>
+                  <c:v>26/01/23</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2081,16 +2081,16 @@
                   <c:v>09/12/2022</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23/12/2022</c:v>
+                  <c:v>30/12/22</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23/01/20232</c:v>
+                  <c:v>23/01/23</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24/01/2023</c:v>
+                  <c:v>25/01/23</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>26/01/2023</c:v>
+                  <c:v>26/01/23</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2111,7 +2111,7 @@
                   <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>43.75</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2184,16 +2184,16 @@
                   <c:v>09/12/2022</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23/12/2022</c:v>
+                  <c:v>30/12/22</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23/01/20232</c:v>
+                  <c:v>23/01/23</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24/01/2023</c:v>
+                  <c:v>25/01/23</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>26/01/2023</c:v>
+                  <c:v>26/01/23</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2285,16 +2285,16 @@
                   <c:v>09/12/2022</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23/12/2022</c:v>
+                  <c:v>30/12/22</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23/01/20232</c:v>
+                  <c:v>23/01/23</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24/01/2023</c:v>
+                  <c:v>25/01/23</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>26/01/2023</c:v>
+                  <c:v>26/01/23</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2627,16 +2627,16 @@
                   <c:v>09/12/2022</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23/12/2022</c:v>
+                  <c:v>30/12/22</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23/01/20232</c:v>
+                  <c:v>23/01/23</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24/01/2023</c:v>
+                  <c:v>25/01/23</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>26/01/2023</c:v>
+                  <c:v>26/01/23</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2657,7 +2657,7 @@
                   <c:v>175</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>450</c:v>
+                  <c:v>406.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1500</c:v>
@@ -2707,16 +2707,16 @@
                   <c:v>09/12/2022</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23/12/2022</c:v>
+                  <c:v>30/12/22</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23/01/20232</c:v>
+                  <c:v>23/01/23</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24/01/2023</c:v>
+                  <c:v>25/01/23</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>26/01/2023</c:v>
+                  <c:v>26/01/23</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2787,16 +2787,16 @@
                   <c:v>09/12/2022</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23/12/2022</c:v>
+                  <c:v>30/12/22</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23/01/20232</c:v>
+                  <c:v>23/01/23</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24/01/2023</c:v>
+                  <c:v>25/01/23</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>26/01/2023</c:v>
+                  <c:v>26/01/23</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2817,7 +2817,7 @@
                   <c:v>175</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>406.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -3250,10 +3250,10 @@
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="25/11/2022" dataDxfId="6" dataCellStyle="Titolo 4"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="05/12/2022" dataDxfId="5" dataCellStyle="Titolo 4"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="09/12/2022" dataDxfId="4" dataCellStyle="Titolo 4"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="23/12/2022" dataDxfId="3" dataCellStyle="Titolo 4"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="23/01/20232" dataDxfId="2" dataCellStyle="Titolo 4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="24/01/2023" dataDxfId="1" dataCellStyle="Titolo 4"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="26/01/2023" dataDxfId="0" dataCellStyle="Titolo 4"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="30/12/22" dataDxfId="3" dataCellStyle="Titolo 4"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="23/01/23" dataDxfId="2" dataCellStyle="Titolo 4"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="25/01/23" dataDxfId="1" dataCellStyle="Titolo 4"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="26/01/23" dataDxfId="0" dataCellStyle="Titolo 4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3554,15 +3554,15 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="25.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.3984375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="52.3984375" customWidth="1"/>
-    <col min="4" max="4" width="33.1328125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="52.5" customWidth="1"/>
+    <col min="4" max="4" width="33.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="65" t="s">
         <v>26</v>
       </c>
@@ -3570,7 +3570,7 @@
       <c r="C1" s="65"/>
       <c r="D1" s="65"/>
     </row>
-    <row r="2" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="64" t="s">
         <v>46</v>
       </c>
@@ -3578,13 +3578,13 @@
       <c r="C2" s="64"/>
       <c r="D2" s="64"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:5" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" s="9" t="s">
         <v>0</v>
       </c>
@@ -3598,7 +3598,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="11" t="s">
         <v>45</v>
       </c>
@@ -3612,7 +3612,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="33" t="s">
         <v>1</v>
       </c>
@@ -3626,7 +3626,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="25.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A7" s="29" t="s">
         <v>2</v>
       </c>
@@ -3640,7 +3640,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="25.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A8" s="34" t="s">
         <v>3</v>
       </c>
@@ -3654,7 +3654,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="25" t="s">
         <v>5</v>
       </c>
@@ -3668,7 +3668,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="38.25" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="42" x14ac:dyDescent="0.15">
       <c r="A10" s="29" t="s">
         <v>4</v>
       </c>
@@ -3683,7 +3683,7 @@
       </c>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" ht="38.25" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="42" x14ac:dyDescent="0.15">
       <c r="A11" s="25" t="s">
         <v>6</v>
       </c>
@@ -3697,7 +3697,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="25.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A12" s="29" t="s">
         <v>7</v>
       </c>
@@ -3711,7 +3711,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="25.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A13" s="35" t="s">
         <v>49</v>
       </c>
@@ -3725,7 +3725,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="38.25" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="42" x14ac:dyDescent="0.15">
       <c r="A14" s="36" t="s">
         <v>50</v>
       </c>
@@ -3739,7 +3739,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="38.25" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="42" x14ac:dyDescent="0.15">
       <c r="A15" s="25" t="s">
         <v>51</v>
       </c>
@@ -3753,7 +3753,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="38.25" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" ht="42" x14ac:dyDescent="0.15">
       <c r="A16" s="29" t="s">
         <v>19</v>
       </c>
@@ -3765,7 +3765,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A17" s="25"/>
       <c r="B17" s="26"/>
       <c r="C17" s="52" t="s">
@@ -3775,7 +3775,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A18" s="29"/>
       <c r="B18" s="23"/>
       <c r="C18" s="53" t="s">
@@ -3785,7 +3785,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A19" s="29"/>
       <c r="B19" s="23"/>
       <c r="C19" s="54" t="s">
@@ -3795,7 +3795,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A20" s="14"/>
       <c r="B20" s="7"/>
       <c r="C20" s="55" t="s">
@@ -3834,27 +3834,27 @@
   </sheetPr>
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="G18" sqref="G18"/>
+      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="41.265625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="18.3984375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="41.33203125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="18.5" style="5" customWidth="1"/>
     <col min="3" max="3" width="19" style="3" customWidth="1"/>
-    <col min="4" max="5" width="19.86328125" style="3" customWidth="1"/>
+    <col min="4" max="5" width="19.83203125" style="3" customWidth="1"/>
     <col min="6" max="6" width="19" style="3" customWidth="1"/>
-    <col min="7" max="7" width="18.73046875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" style="3" customWidth="1"/>
     <col min="8" max="8" width="20" style="3" customWidth="1"/>
-    <col min="9" max="9" width="19.265625" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="8.86328125" style="3"/>
+    <col min="9" max="9" width="19.33203125" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="66" t="s">
         <v>26</v>
       </c>
@@ -3866,7 +3866,7 @@
       <c r="G1" s="66"/>
       <c r="H1" s="66"/>
     </row>
-    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="58" t="s">
         <v>80</v>
       </c>
@@ -3893,7 +3893,7 @@
       </c>
       <c r="I2" s="56"/>
     </row>
-    <row r="3" spans="1:9" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:9" ht="20" x14ac:dyDescent="0.25">
       <c r="A3" s="37" t="s">
         <v>0</v>
       </c>
@@ -3919,7 +3919,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="38" t="s">
         <v>37</v>
       </c>
@@ -3945,7 +3945,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="41" t="s">
         <v>30</v>
       </c>
@@ -3971,7 +3971,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="41" t="s">
         <v>32</v>
       </c>
@@ -3985,7 +3985,7 @@
         <v>50</v>
       </c>
       <c r="E6" s="39">
-        <v>0</v>
+        <v>43.75</v>
       </c>
       <c r="F6" s="39">
         <v>0</v>
@@ -3997,7 +3997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="41" t="s">
         <v>31</v>
       </c>
@@ -4023,7 +4023,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="41" t="s">
         <v>69</v>
       </c>
@@ -4037,7 +4037,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="59">
         <v>0</v>
@@ -4049,7 +4049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="42" t="s">
         <v>33</v>
       </c>
@@ -4067,7 +4067,7 @@
       </c>
       <c r="E9" s="60">
         <f t="shared" si="0"/>
-        <v>450</v>
+        <v>406.25</v>
       </c>
       <c r="F9" s="60">
         <f t="shared" si="0"/>
@@ -4082,7 +4082,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="42" t="s">
         <v>34</v>
       </c>
@@ -4115,7 +4115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="43" t="s">
         <v>35</v>
       </c>
@@ -4131,9 +4131,9 @@
         <f t="shared" si="2"/>
         <v>4.5</v>
       </c>
-      <c r="E11" s="60" t="str">
+      <c r="E11" s="60">
         <f t="shared" si="2"/>
-        <v/>
+        <v>10.285714285714286</v>
       </c>
       <c r="F11" s="60" t="str">
         <f t="shared" si="2"/>
@@ -4148,7 +4148,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="44" t="s">
         <v>36</v>
       </c>
@@ -4181,7 +4181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="45" t="s">
         <v>64</v>
       </c>
@@ -4197,9 +4197,9 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E13" s="60" t="str">
+      <c r="E13" s="60">
         <f t="shared" si="4"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="F13" s="60" t="str">
         <f t="shared" si="4"/>
@@ -4214,7 +4214,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="45" t="s">
         <v>65</v>
       </c>
@@ -4230,9 +4230,9 @@
         <f t="shared" si="5"/>
         <v>50</v>
       </c>
-      <c r="E14" s="60" t="str">
+      <c r="E14" s="60">
         <f t="shared" si="5"/>
-        <v/>
+        <v>43.75</v>
       </c>
       <c r="F14" s="60" t="str">
         <f t="shared" si="5"/>
@@ -4247,7 +4247,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="45" t="s">
         <v>66</v>
       </c>
@@ -4263,9 +4263,9 @@
         <f t="shared" si="6"/>
         <v>175</v>
       </c>
-      <c r="E15" s="60" t="str">
+      <c r="E15" s="60">
         <f t="shared" si="6"/>
-        <v/>
+        <v>406.25</v>
       </c>
       <c r="F15" s="60" t="str">
         <f t="shared" si="6"/>
@@ -4280,7 +4280,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="14.25" hidden="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="46" t="s">
         <v>25</v>
       </c>
@@ -4296,9 +4296,9 @@
         <f t="shared" si="7"/>
         <v>2.75</v>
       </c>
-      <c r="E16" s="47" t="e">
+      <c r="E16" s="47">
         <f t="shared" si="7"/>
-        <v>#VALUE!</v>
+        <v>5.6428571428571432</v>
       </c>
       <c r="F16" s="47" t="e">
         <f t="shared" si="7"/>
@@ -4313,7 +4313,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="14.25" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" ht="16" x14ac:dyDescent="0.15">
       <c r="A17" s="48" t="s">
         <v>71</v>
       </c>
@@ -4331,7 +4331,7 @@
       </c>
       <c r="E17" s="50" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>GREEN</v>
       </c>
       <c r="F17" s="51" t="str">
         <f t="shared" si="8"/>
@@ -4346,108 +4346,108 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.15">
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:6" x14ac:dyDescent="0.15">
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
     </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="3:6" x14ac:dyDescent="0.15">
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
     </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:6" x14ac:dyDescent="0.15">
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
@@ -4512,11 +4512,11 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="Y67" sqref="Y67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -4536,6 +4536,19 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <documentManagement>
     <NumericAssetId xmlns="145c5697-5eb5-440b-b2f1-a8273fb59250" xsi:nil="true"/>
@@ -4548,7 +4561,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="OOFile" ma:contentTypeID="0x0101006025706CF4CD034688BEBAE97A2E701D020200C3831ACA17D8814887A164412888521E" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ed1fea5d08807278759d338940aa9e8f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="145c5697-5eb5-440b-b2f1-a8273fb59250" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="174e4b03d57b3d621fa064bbab783e99" ns2:_="">
     <xsd:import namespace="145c5697-5eb5-440b-b2f1-a8273fb59250"/>
@@ -4705,20 +4718,23 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C8952B8-A92A-4EC6-919A-585326AE1665}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{59DE95EC-569D-4A4A-A6C6-CE9D2601D3CE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C132233-F222-492C-9D45-2E862E9A3BD7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -4727,7 +4743,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{114F2242-DD79-4927-A859-E00403A130D8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4743,20 +4759,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C8952B8-A92A-4EC6-919A-585326AE1665}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{59DE95EC-569D-4A4A-A6C6-CE9D2601D3CE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Final EVM and Status Report
</commit_message>
<xml_diff>
--- a/Documenti/EVM/GreenLeaf_EVM.xlsx
+++ b/Documenti/EVM/GreenLeaf_EVM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10116"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anton\Documents\GitHub\Green-Leaf\Documenti\EVM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antoniogiametta/Documents/GitHub/Green-Leaf/Documenti/EVM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D82CAB6-83ED-4865-AB0C-87B7E020DB2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{761E1677-6716-6C46-8CD0-153FC04B773A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="261" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="261" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="definizioni" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="90">
   <si>
     <t>Metric</t>
   </si>
@@ -307,16 +307,19 @@
     <t>30/12/22</t>
   </si>
   <si>
-    <t>23/01/23</t>
-  </si>
-  <si>
-    <t>25/01/23</t>
-  </si>
-  <si>
-    <t>26/01/23</t>
-  </si>
-  <si>
     <t>17/01/2023</t>
+  </si>
+  <si>
+    <t>31/01/23</t>
+  </si>
+  <si>
+    <t>05/02/23</t>
+  </si>
+  <si>
+    <t>09/02/23</t>
+  </si>
+  <si>
+    <t>Final</t>
   </si>
 </sst>
 </file>
@@ -737,7 +740,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -926,6 +929,21 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="10" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -937,19 +955,7 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="10" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -962,95 +968,6 @@
     <cellStyle name="Titolo 4" xfId="2" builtinId="19"/>
   </cellStyles>
   <dxfs count="18">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="9"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="16"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="18"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="26"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="43"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="57"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="9"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="10"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="16"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="43"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor indexed="58"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;€&quot;\ #,##0.00"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1157,6 +1074,11 @@
           <color indexed="64"/>
         </bottom>
       </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;€&quot;\ #,##0.00"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
@@ -1395,6 +1317,90 @@
       </border>
       <protection locked="0" hidden="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="16"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="18"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="26"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="43"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="57"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="9"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="10"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="16"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="13"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="43"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="58"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -1573,13 +1579,13 @@
                   <c:v>17/01/2023</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>23/01/23</c:v>
+                  <c:v>31/01/23</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>25/01/23</c:v>
+                  <c:v>05/02/23</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>26/01/23</c:v>
+                  <c:v>09/02/23</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1603,16 +1609,16 @@
                   <c:v>10.285714285714286</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.4285714285714284</c:v>
+                  <c:v>5.7142857142857144</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.59523809523809523</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>0.47363435427849704</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1682,13 +1688,13 @@
                   <c:v>17/01/2023</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>23/01/23</c:v>
+                  <c:v>31/01/23</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>25/01/23</c:v>
+                  <c:v>05/02/23</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>26/01/23</c:v>
+                  <c:v>09/02/23</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1712,16 +1718,16 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.6</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2032,13 +2038,13 @@
                   <c:v>17/01/2023</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>23/01/23</c:v>
+                  <c:v>31/01/23</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>25/01/23</c:v>
+                  <c:v>05/02/23</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>26/01/23</c:v>
+                  <c:v>09/02/23</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2141,13 +2147,13 @@
                   <c:v>17/01/2023</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>23/01/23</c:v>
+                  <c:v>31/01/23</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>25/01/23</c:v>
+                  <c:v>05/02/23</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>26/01/23</c:v>
+                  <c:v>09/02/23</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2174,13 +2180,13 @@
                   <c:v>131.25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1260</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>158.35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2250,13 +2256,13 @@
                   <c:v>17/01/2023</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>23/01/23</c:v>
+                  <c:v>31/01/23</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>25/01/23</c:v>
+                  <c:v>05/02/23</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>26/01/23</c:v>
+                  <c:v>09/02/23</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2280,16 +2286,16 @@
                   <c:v>450</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>450</c:v>
+                  <c:v>750</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>750</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>225</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2357,13 +2363,13 @@
                   <c:v>17/01/2023</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>23/01/23</c:v>
+                  <c:v>31/01/23</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>25/01/23</c:v>
+                  <c:v>05/02/23</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>26/01/23</c:v>
+                  <c:v>09/02/23</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2705,13 +2711,13 @@
                   <c:v>17/01/2023</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>23/01/23</c:v>
+                  <c:v>31/01/23</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>25/01/23</c:v>
+                  <c:v>05/02/23</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>26/01/23</c:v>
+                  <c:v>09/02/23</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2735,16 +2741,16 @@
                   <c:v>406.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>318.75</c:v>
+                  <c:v>618.75</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-131.25</c:v>
+                  <c:v>-510</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>-75</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>-83.35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2791,13 +2797,13 @@
                   <c:v>17/01/2023</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>23/01/23</c:v>
+                  <c:v>31/01/23</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>25/01/23</c:v>
+                  <c:v>05/02/23</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>26/01/23</c:v>
+                  <c:v>09/02/23</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2821,16 +2827,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-300</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-750</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-225</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-75</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2877,13 +2883,13 @@
                   <c:v>17/01/2023</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>23/01/23</c:v>
+                  <c:v>31/01/23</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>25/01/23</c:v>
+                  <c:v>05/02/23</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>26/01/23</c:v>
+                  <c:v>09/02/23</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2907,16 +2913,16 @@
                   <c:v>406.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>531.25</c:v>
+                  <c:v>618.75</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>-510</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>-75</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>-83.35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3333,18 +3339,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabella1" displayName="Tabella1" ref="A3:I17" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16" tableBorderDxfId="15" headerRowCellStyle="Titolo 4" dataCellStyle="Titolo 4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabella1" displayName="Tabella1" ref="A3:I17" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" tableBorderDxfId="9" headerRowCellStyle="Titolo 4" dataCellStyle="Titolo 4">
   <autoFilter ref="A3:I17" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Metric" dataDxfId="14" dataCellStyle="Titolo 4"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="25/11/2022" dataDxfId="13" dataCellStyle="Titolo 4"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="05/12/2022" dataDxfId="12" dataCellStyle="Titolo 4"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="09/12/2022" dataDxfId="11" dataCellStyle="Titolo 4"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="30/12/22" dataDxfId="10" dataCellStyle="Titolo 4"/>
-    <tableColumn id="9" xr3:uid="{2A10284F-2DC8-4F45-B2E9-3DFB9B094230}" name="17/01/2023" dataDxfId="6" dataCellStyle="Output"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="23/01/23" dataDxfId="9" dataCellStyle="Titolo 4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="25/01/23" dataDxfId="8" dataCellStyle="Titolo 4"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="26/01/23" dataDxfId="7" dataCellStyle="Titolo 4"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Metric" dataDxfId="8" dataCellStyle="Titolo 4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="25/11/2022" dataDxfId="7" dataCellStyle="Titolo 4"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="05/12/2022" dataDxfId="6" dataCellStyle="Titolo 4"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="09/12/2022" dataDxfId="5" dataCellStyle="Titolo 4"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="30/12/22" dataDxfId="4" dataCellStyle="Titolo 4"/>
+    <tableColumn id="9" xr3:uid="{2A10284F-2DC8-4F45-B2E9-3DFB9B094230}" name="17/01/2023" dataDxfId="3" dataCellStyle="Output"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="31/01/23" dataDxfId="2" dataCellStyle="Titolo 4"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="05/02/23" dataDxfId="1" dataCellStyle="Titolo 4"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="09/02/23" dataDxfId="0" dataCellStyle="Titolo 4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3645,37 +3651,37 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="52.42578125" customWidth="1"/>
-    <col min="4" max="4" width="33.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="52.5" customWidth="1"/>
+    <col min="4" max="4" width="33.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="s">
+    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-    </row>
-    <row r="2" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="64" t="s">
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+    </row>
+    <row r="2" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="68" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" s="9" t="s">
         <v>0</v>
       </c>
@@ -3689,7 +3695,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="11" t="s">
         <v>45</v>
       </c>
@@ -3703,7 +3709,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="33" t="s">
         <v>1</v>
       </c>
@@ -3717,7 +3723,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A7" s="29" t="s">
         <v>2</v>
       </c>
@@ -3731,7 +3737,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A8" s="34" t="s">
         <v>3</v>
       </c>
@@ -3745,7 +3751,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="25" t="s">
         <v>5</v>
       </c>
@@ -3759,7 +3765,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="42" x14ac:dyDescent="0.15">
       <c r="A10" s="29" t="s">
         <v>4</v>
       </c>
@@ -3774,7 +3780,7 @@
       </c>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="42" x14ac:dyDescent="0.15">
       <c r="A11" s="25" t="s">
         <v>6</v>
       </c>
@@ -3788,7 +3794,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A12" s="29" t="s">
         <v>7</v>
       </c>
@@ -3802,7 +3808,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A13" s="35" t="s">
         <v>49</v>
       </c>
@@ -3816,7 +3822,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="42" x14ac:dyDescent="0.15">
       <c r="A14" s="36" t="s">
         <v>50</v>
       </c>
@@ -3830,7 +3836,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="42" x14ac:dyDescent="0.15">
       <c r="A15" s="25" t="s">
         <v>51</v>
       </c>
@@ -3844,7 +3850,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="42" x14ac:dyDescent="0.15">
       <c r="A16" s="29" t="s">
         <v>19</v>
       </c>
@@ -3856,7 +3862,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A17" s="25"/>
       <c r="B17" s="26"/>
       <c r="C17" s="52" t="s">
@@ -3866,7 +3872,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A18" s="29"/>
       <c r="B18" s="23"/>
       <c r="C18" s="53" t="s">
@@ -3876,7 +3882,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A19" s="29"/>
       <c r="B19" s="23"/>
       <c r="C19" s="54" t="s">
@@ -3886,7 +3892,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="14" x14ac:dyDescent="0.15">
       <c r="A20" s="14"/>
       <c r="B20" s="7"/>
       <c r="C20" s="55" t="s">
@@ -3923,42 +3929,42 @@
     <tabColor indexed="19"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C28" sqref="C28"/>
+      <selection pane="bottomRight" activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="41.28515625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="41.33203125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="18.5" style="5" customWidth="1"/>
     <col min="3" max="3" width="19" style="3" customWidth="1"/>
-    <col min="4" max="6" width="19.85546875" style="3" customWidth="1"/>
+    <col min="4" max="6" width="19.83203125" style="3" customWidth="1"/>
     <col min="7" max="7" width="19" style="3" customWidth="1"/>
-    <col min="8" max="8" width="18.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" style="3" customWidth="1"/>
     <col min="9" max="9" width="20" style="3" customWidth="1"/>
-    <col min="10" max="10" width="19.28515625" style="3" customWidth="1"/>
-    <col min="11" max="16384" width="8.85546875" style="3"/>
+    <col min="10" max="10" width="19.33203125" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="66" t="s">
+    <row r="1" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="70" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-    </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="58" t="s">
         <v>80</v>
       </c>
@@ -3988,7 +3994,7 @@
       </c>
       <c r="J2" s="56"/>
     </row>
-    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="20" x14ac:dyDescent="0.25">
       <c r="A3" s="37" t="s">
         <v>0</v>
       </c>
@@ -4005,19 +4011,22 @@
         <v>84</v>
       </c>
       <c r="F3" s="63" t="s">
+        <v>85</v>
+      </c>
+      <c r="G3" s="63" t="s">
+        <v>86</v>
+      </c>
+      <c r="H3" s="63" t="s">
+        <v>87</v>
+      </c>
+      <c r="I3" s="63" t="s">
         <v>88</v>
       </c>
-      <c r="G3" s="63" t="s">
-        <v>85</v>
-      </c>
-      <c r="H3" s="63" t="s">
-        <v>86</v>
-      </c>
-      <c r="I3" s="63" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="K3" s="71" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="38" t="s">
         <v>37</v>
       </c>
@@ -4045,8 +4054,12 @@
       <c r="I4" s="39">
         <v>75</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="K4" s="3">
+        <f>SUM(Tabella1[[#This Row],[25/11/2022]:[09/02/23]])</f>
+        <v>3750</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="41" t="s">
         <v>30</v>
       </c>
@@ -4068,22 +4081,26 @@
       </c>
       <c r="F5" s="39">
         <f t="shared" si="0"/>
-        <v>450</v>
+        <v>750</v>
       </c>
       <c r="G5" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>750</v>
       </c>
       <c r="H5" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>225</v>
       </c>
       <c r="I5" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="K5" s="3">
+        <f>SUM(Tabella1[[#This Row],[25/11/2022]:[09/02/23]])</f>
+        <v>3750</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="41" t="s">
         <v>32</v>
       </c>
@@ -4102,17 +4119,21 @@
       <c r="F6" s="39">
         <v>131.25</v>
       </c>
-      <c r="G6" s="68">
-        <v>0</v>
+      <c r="G6" s="65">
+        <v>1260</v>
       </c>
       <c r="H6" s="40">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="I6" s="40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+        <v>158.35</v>
+      </c>
+      <c r="K6" s="3">
+        <f>SUM(Tabella1[[#This Row],[25/11/2022]:[09/02/23]])</f>
+        <v>2877.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="41" t="s">
         <v>31</v>
       </c>
@@ -4140,8 +4161,12 @@
       <c r="I7" s="39">
         <v>75</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="K7" s="3">
+        <f>SUM(Tabella1[[#This Row],[25/11/2022]:[09/02/23]])</f>
+        <v>3750</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="41" t="s">
         <v>69</v>
       </c>
@@ -4158,19 +4183,19 @@
         <v>1</v>
       </c>
       <c r="F8" s="59">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="G8" s="59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" s="59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" s="59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="42" t="s">
         <v>33</v>
       </c>
@@ -4192,22 +4217,26 @@
       </c>
       <c r="F9" s="60">
         <f t="shared" ref="F9" si="2">F5-F6</f>
-        <v>318.75</v>
+        <v>618.75</v>
       </c>
       <c r="G9" s="60">
-        <f>G5-F6</f>
-        <v>-131.25</v>
+        <f>G5-G6</f>
+        <v>-510</v>
       </c>
       <c r="H9" s="60">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-75</v>
       </c>
       <c r="I9" s="60">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+        <v>-83.35</v>
+      </c>
+      <c r="K9" s="3">
+        <f>K5-K6</f>
+        <v>872.90000000000009</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="42" t="s">
         <v>34</v>
       </c>
@@ -4229,22 +4258,22 @@
       </c>
       <c r="F10" s="60">
         <f t="shared" ref="F10" si="4">F5-F7</f>
-        <v>-300</v>
+        <v>0</v>
       </c>
       <c r="G10" s="60">
         <f t="shared" si="3"/>
-        <v>-750</v>
+        <v>0</v>
       </c>
       <c r="H10" s="60">
         <f t="shared" si="3"/>
-        <v>-225</v>
+        <v>0</v>
       </c>
       <c r="I10" s="60">
         <f t="shared" si="3"/>
-        <v>-75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="43" t="s">
         <v>35</v>
       </c>
@@ -4266,22 +4295,26 @@
       </c>
       <c r="F11" s="60">
         <f t="shared" ref="F11" si="6">IF(F6,F5/F6,"")</f>
-        <v>3.4285714285714284</v>
+        <v>5.7142857142857144</v>
       </c>
       <c r="G11" s="60">
-        <f>IF(F6,G5/F6,"")</f>
-        <v>0</v>
-      </c>
-      <c r="H11" s="60" t="str">
+        <f>IF(G6,G5/G6,"")</f>
+        <v>0.59523809523809523</v>
+      </c>
+      <c r="H11" s="60">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="I11" s="60" t="str">
+        <v>0.75</v>
+      </c>
+      <c r="I11" s="60">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0.47363435427849704</v>
+      </c>
+      <c r="K11" s="3">
+        <f>K5/K6</f>
+        <v>1.3033957804733933</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="44" t="s">
         <v>36</v>
       </c>
@@ -4303,22 +4336,26 @@
       </c>
       <c r="F12" s="60">
         <f t="shared" ref="F12" si="8">IF(F7,F5/F7,"")</f>
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="G12" s="60">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" s="60">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12" s="60">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="K12" s="3">
+        <f>K5/K7</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="45" t="s">
         <v>64</v>
       </c>
@@ -4340,22 +4377,22 @@
       </c>
       <c r="F13" s="60">
         <f t="shared" ref="F13" si="10">IF(F5,IF(F6,F14-F6,""),"")</f>
-        <v>87.5</v>
-      </c>
-      <c r="G13" s="60" t="str">
+        <v>0</v>
+      </c>
+      <c r="G13" s="60">
         <f>IF(G5,IF(F6,G14-F6,""),"")</f>
-        <v/>
-      </c>
-      <c r="H13" s="60" t="str">
+        <v>1128.75</v>
+      </c>
+      <c r="H13" s="60">
         <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="I13" s="60" t="str">
+        <v>0</v>
+      </c>
+      <c r="I13" s="60">
         <f t="shared" si="9"/>
-        <v/>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="45" t="s">
         <v>65</v>
       </c>
@@ -4377,22 +4414,22 @@
       </c>
       <c r="F14" s="60">
         <f t="shared" ref="F14" si="12">IF(F5,IF(F6,F4/F11,""),"")</f>
-        <v>218.75</v>
-      </c>
-      <c r="G14" s="60" t="str">
+        <v>131.25</v>
+      </c>
+      <c r="G14" s="60">
         <f>IF(G5,IF(F6,G4/G11,""),"")</f>
-        <v/>
-      </c>
-      <c r="H14" s="60" t="str">
+        <v>1260</v>
+      </c>
+      <c r="H14" s="60">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="I14" s="60" t="str">
+        <v>300</v>
+      </c>
+      <c r="I14" s="60">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+        <v>158.35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="45" t="s">
         <v>66</v>
       </c>
@@ -4414,22 +4451,22 @@
       </c>
       <c r="F15" s="60">
         <f t="shared" ref="F15" si="14">IF(F5,IF(F6,F4-F14,""),"")</f>
-        <v>531.25</v>
-      </c>
-      <c r="G15" s="60" t="str">
+        <v>618.75</v>
+      </c>
+      <c r="G15" s="60">
         <f>IF(G5,IF(F6,G4-G14,""),"")</f>
-        <v/>
-      </c>
-      <c r="H15" s="60" t="str">
+        <v>-510</v>
+      </c>
+      <c r="H15" s="60">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="I15" s="60" t="str">
+        <v>-75</v>
+      </c>
+      <c r="I15" s="60">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="15" hidden="1" x14ac:dyDescent="0.25">
+        <v>-83.35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="46" t="s">
         <v>25</v>
       </c>
@@ -4452,18 +4489,18 @@
       <c r="F16" s="47"/>
       <c r="G16" s="47">
         <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="H16" s="47" t="e">
+        <v>0.79761904761904767</v>
+      </c>
+      <c r="H16" s="47">
         <f t="shared" si="15"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I16" s="47" t="e">
+        <v>0.875</v>
+      </c>
+      <c r="I16" s="47">
         <f t="shared" si="15"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+        <v>0.73681717713924855</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="16" x14ac:dyDescent="0.15">
       <c r="A17" s="48" t="s">
         <v>71</v>
       </c>
@@ -4486,138 +4523,138 @@
       <c r="F17" s="50"/>
       <c r="G17" s="51" t="str">
         <f>IF(G7,IF(F6,IF(G16&lt;0.65,"BLACK",IF(G16&lt;0.85,"RED",IF(G16&lt;1,"YELLOW","GREEN"))),""),"")</f>
-        <v>BLACK</v>
+        <v>RED</v>
       </c>
       <c r="H17" s="51" t="str">
         <f t="shared" si="16"/>
-        <v/>
+        <v>YELLOW</v>
       </c>
       <c r="I17" s="51" t="str">
         <f t="shared" si="16"/>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+        <v>RED</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="G20" s="5"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B22" s="69"/>
-      <c r="C22" s="69"/>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B22" s="66"/>
+      <c r="C22" s="66"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B23" s="69"/>
-      <c r="C23" s="69"/>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B23" s="66"/>
+      <c r="C23" s="66"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B25" s="70"/>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B25" s="67"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
-      <c r="G26" s="67"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G26" s="64"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
     </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
     </row>
-    <row r="34" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
     </row>
-    <row r="35" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="3:7" x14ac:dyDescent="0.15">
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
@@ -4631,24 +4668,24 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A17">
-    <cfRule type="cellIs" dxfId="5" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="1" stopIfTrue="1" operator="equal">
       <formula>"GREEN"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="2" stopIfTrue="1" operator="equal">
       <formula>"YELLOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="3" stopIfTrue="1" operator="equal">
       <formula>"RED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:I17">
-    <cfRule type="cellIs" dxfId="2" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="4" stopIfTrue="1" operator="equal">
       <formula>"GREEN"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="5" stopIfTrue="1" operator="equal">
       <formula>"YELLOW"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="6" stopIfTrue="1" operator="equal">
       <formula>"RED"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4683,11 +4720,11 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="Y67" sqref="Y67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -4707,19 +4744,19 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <NumericAssetId xmlns="145c5697-5eb5-440b-b2f1-a8273fb59250" xsi:nil="true"/>
+    <AssetType xmlns="145c5697-5eb5-440b-b2f1-a8273fb59250">TP</AssetType>
+    <Markets xmlns="145c5697-5eb5-440b-b2f1-a8273fb59250" xsi:nil="true"/>
+    <AppVer xmlns="145c5697-5eb5-440b-b2f1-a8273fb59250" xsi:nil="true"/>
+    <AuthoringAssetId xmlns="145c5697-5eb5-440b-b2f1-a8273fb59250">TP001142302</AuthoringAssetId>
+    <AssetId xmlns="145c5697-5eb5-440b-b2f1-a8273fb59250">TS001142302</AssetId>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="OOFile" ma:contentTypeID="0x0101006025706CF4CD034688BEBAE97A2E701D020200C3831ACA17D8814887A164412888521E" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ed1fea5d08807278759d338940aa9e8f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="145c5697-5eb5-440b-b2f1-a8273fb59250" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="174e4b03d57b3d621fa064bbab783e99" ns2:_="">
     <xsd:import namespace="145c5697-5eb5-440b-b2f1-a8273fb59250"/>
@@ -4876,36 +4913,29 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <NumericAssetId xmlns="145c5697-5eb5-440b-b2f1-a8273fb59250" xsi:nil="true"/>
-    <AssetType xmlns="145c5697-5eb5-440b-b2f1-a8273fb59250">TP</AssetType>
-    <Markets xmlns="145c5697-5eb5-440b-b2f1-a8273fb59250" xsi:nil="true"/>
-    <AppVer xmlns="145c5697-5eb5-440b-b2f1-a8273fb59250" xsi:nil="true"/>
-    <AuthoringAssetId xmlns="145c5697-5eb5-440b-b2f1-a8273fb59250">TP001142302</AuthoringAssetId>
-    <AssetId xmlns="145c5697-5eb5-440b-b2f1-a8273fb59250">TS001142302</AssetId>
-  </documentManagement>
-</p:properties>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{59DE95EC-569D-4A4A-A6C6-CE9D2601D3CE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C132233-F222-492C-9D45-2E862E9A3BD7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="145c5697-5eb5-440b-b2f1-a8273fb59250"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C8952B8-A92A-4EC6-919A-585326AE1665}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{114F2242-DD79-4927-A859-E00403A130D8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4923,11 +4953,18 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C8952B8-A92A-4EC6-919A-585326AE1665}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C132233-F222-492C-9D45-2E862E9A3BD7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{59DE95EC-569D-4A4A-A6C6-CE9D2601D3CE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="145c5697-5eb5-440b-b2f1-a8273fb59250"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>